<commit_message>
Excel datasource now handles null cells and missing id column
</commit_message>
<xml_diff>
--- a/src/OpenDataService.Tests/data/excelfile.xlsx
+++ b/src/OpenDataService.Tests/data/excelfile.xlsx
@@ -5,11 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Tab1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Set2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="nulls" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="missingId" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -69,6 +71,12 @@
   </si>
   <si>
     <t xml:space="preserve">The quick brown fox jumps over the lazy dog</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
   </si>
 </sst>
 </file>
@@ -180,7 +188,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -240,11 +248,11 @@
   </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -312,6 +320,118 @@
       </c>
       <c r="E4" s="2" t="n">
         <v>0.098</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>